<commit_message>
Application Import error management - Fix junit
</commit_message>
<xml_diff>
--- a/src/test/resources/junit/application_import/02-import-applications-name-changed.xlsx
+++ b/src/test/resources/junit/application_import/02-import-applications-name-changed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lionelcoquin/development/ea-design-it/src/test/resources/junit/application_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D4BC71-ACD1-7F4E-92DB-78C39C1394BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22244E60-B17B-4B41-B6EA-9CAEE595383D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>application.id</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Description 0005</t>
+  </si>
+  <si>
+    <t>Jean</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1039,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1069,8 +1072,8 @@
       <c r="A3" t="s">
         <v>57</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>

</xml_diff>